<commit_message>
commit dos arquivos alterados
</commit_message>
<xml_diff>
--- a/dados/exp_algas.xlsx
+++ b/dados/exp_algas.xlsx
@@ -24,10 +24,10 @@
     <t>Y</t>
   </si>
   <si>
-    <t>tratament</t>
+    <t>control</t>
   </si>
   <si>
-    <t>control</t>
+    <t>treatment</t>
   </si>
 </sst>
 </file>
@@ -368,7 +368,7 @@
   <dimension ref="B2:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -389,7 +389,7 @@
     </row>
     <row r="3" spans="2:4">
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>5</v>
@@ -398,7 +398,7 @@
     </row>
     <row r="4" spans="2:4">
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -407,7 +407,7 @@
     </row>
     <row r="5" spans="2:4">
       <c r="B5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -416,7 +416,7 @@
     </row>
     <row r="6" spans="2:4">
       <c r="B6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -425,7 +425,7 @@
     </row>
     <row r="7" spans="2:4">
       <c r="B7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>11</v>
@@ -434,7 +434,7 @@
     </row>
     <row r="8" spans="2:4">
       <c r="B8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -443,7 +443,7 @@
     </row>
     <row r="9" spans="2:4">
       <c r="B9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>6</v>
@@ -452,7 +452,7 @@
     </row>
     <row r="10" spans="2:4">
       <c r="B10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -461,7 +461,7 @@
     </row>
     <row r="11" spans="2:4">
       <c r="B11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -470,7 +470,7 @@
     </row>
     <row r="12" spans="2:4">
       <c r="B12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -479,7 +479,7 @@
     </row>
     <row r="13" spans="2:4">
       <c r="B13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>3</v>
@@ -488,7 +488,7 @@
     </row>
     <row r="14" spans="2:4">
       <c r="B14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -497,7 +497,7 @@
     </row>
     <row r="15" spans="2:4">
       <c r="B15" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>11</v>
@@ -506,7 +506,7 @@
     </row>
     <row r="16" spans="2:4">
       <c r="B16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -515,7 +515,7 @@
     </row>
     <row r="17" spans="2:4">
       <c r="B17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>9</v>
@@ -524,7 +524,7 @@
     </row>
     <row r="18" spans="2:4">
       <c r="B18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18">
         <v>3</v>
@@ -533,7 +533,7 @@
     </row>
     <row r="19" spans="2:4">
       <c r="B19" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>12</v>
@@ -542,7 +542,7 @@
     </row>
     <row r="20" spans="2:4">
       <c r="B20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="21" spans="2:4">
       <c r="B21" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C21">
         <v>13</v>
@@ -560,7 +560,7 @@
     </row>
     <row r="22" spans="2:4">
       <c r="B22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22">
         <v>6</v>
@@ -569,7 +569,7 @@
     </row>
     <row r="23" spans="2:4">
       <c r="B23" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -577,7 +577,7 @@
     </row>
     <row r="24" spans="2:4">
       <c r="B24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24">
         <v>2</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="25" spans="2:4">
       <c r="B25" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -593,7 +593,7 @@
     </row>
     <row r="26" spans="2:4">
       <c r="B26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -601,7 +601,7 @@
     </row>
     <row r="27" spans="2:4">
       <c r="B27" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27">
         <v>7</v>
@@ -609,7 +609,7 @@
     </row>
     <row r="28" spans="2:4">
       <c r="B28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -617,7 +617,7 @@
     </row>
     <row r="29" spans="2:4">
       <c r="B29" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C29">
         <v>7</v>
@@ -625,7 +625,7 @@
     </row>
     <row r="30" spans="2:4">
       <c r="B30" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -633,7 +633,7 @@
     </row>
     <row r="31" spans="2:4">
       <c r="B31" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -641,7 +641,7 @@
     </row>
     <row r="32" spans="2:4">
       <c r="B32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -649,7 +649,7 @@
     </row>
     <row r="33" spans="2:3">
       <c r="B33" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C33">
         <v>7</v>
@@ -657,7 +657,7 @@
     </row>
     <row r="34" spans="2:3">
       <c r="B34" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="35" spans="2:3">
       <c r="B35" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C35">
         <v>4</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="36" spans="2:3">
       <c r="B36" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C36">
         <v>0</v>
@@ -681,7 +681,7 @@
     </row>
     <row r="37" spans="2:3">
       <c r="B37" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C37">
         <v>4</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="38" spans="2:3">
       <c r="B38" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -697,7 +697,7 @@
     </row>
     <row r="39" spans="2:3">
       <c r="B39" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C39">
         <v>1</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="40" spans="2:3">
       <c r="B40" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C40">
         <v>0</v>
@@ -713,7 +713,7 @@
     </row>
     <row r="41" spans="2:3">
       <c r="B41" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C41">
         <v>4</v>
@@ -721,7 +721,7 @@
     </row>
     <row r="42" spans="2:3">
       <c r="B42" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C42">
         <v>1</v>

</xml_diff>